<commit_message>
Java (Eclipse IDE), con Selenium webdriver, TestNG, Maven, Apache Poi (Manipulacion de matrices de datos a partir de archivos excel) reportes automatizados con Extent Reports
</commit_message>
<xml_diff>
--- a/TestBPM/DataProvider/inputData.xlsx
+++ b/TestBPM/DataProvider/inputData.xlsx
@@ -635,6 +635,7 @@
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="N4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -717,9 +718,7 @@
       <c r="M6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="N6" t="s">
-        <v>47</v>
-      </c>
+      <c r="N6"/>
     </row>
     <row customFormat="1" r="7" s="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">

</xml_diff>